<commit_message>
Inspection of songs signatures
</commit_message>
<xml_diff>
--- a/dataset/songs_with_signature_and_length.xlsx
+++ b/dataset/songs_with_signature_and_length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\GitHub\Tresillo\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F1CE23-A0C3-486C-824C-56A172ED02A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08911EA6-1F62-4AB8-9C8B-D5C426959D5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3171,7 +3171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3187,13 +3187,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -3220,48 +3244,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -3297,6 +3298,35 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3311,10 +3341,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1BC977F-93A7-4443-B601-8EA545A39641}" name="Tabelle1" displayName="Tabelle1" ref="A1:D443" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D443" xr:uid="{5A276807-760A-4EC0-83F2-9F298F09E7B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1BC977F-93A7-4443-B601-8EA545A39641}" name="Tabelle1" displayName="Tabelle1" ref="A1:D443" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:D443" xr:uid="{5A276807-760A-4EC0-83F2-9F298F09E7B0}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="{1: '3/4'}"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3CEE1EE4-0D26-42C5-A48C-B12CDA406857}" name="Spalte1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3CEE1EE4-0D26-42C5-A48C-B12CDA406857}" name="Spalte1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{47DDDC08-2AC3-45A5-9617-9D22A1D9ADF8}" name="name"/>
     <tableColumn id="3" xr3:uid="{E164C516-5ABF-4B21-BF6A-A3B86732B5F9}" name="time signature"/>
     <tableColumn id="4" xr3:uid="{9F6F8FEA-82DE-47CD-AE60-643353A5BBE7}" name="length"/>
@@ -3644,16 +3680,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D443"/>
+  <dimension ref="A1:E443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C58" sqref="C1:C1048576"/>
+      <selection activeCell="E431" sqref="E431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="157.85546875" customWidth="1"/>
+    <col min="2" max="2" width="182.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3671,7 +3707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3685,7 +3721,7 @@
         <v>48.061291868749997</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3699,7 +3735,7 @@
         <v>29.443490075</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3713,7 +3749,7 @@
         <v>56.999943000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3727,7 +3763,7 @@
         <v>34.973568802083342</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3741,7 +3777,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3755,7 +3791,7 @@
         <v>28.664648006250001</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3769,7 +3805,7 @@
         <v>48.489822375000003</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3783,7 +3819,7 @@
         <v>34.907842374999987</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3797,7 +3833,7 @@
         <v>44.95713096875</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3811,7 +3847,7 @@
         <v>37.6363275</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3825,7 +3861,7 @@
         <v>45.003978983333333</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3839,7 +3875,7 @@
         <v>41.655262875000012</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3853,7 +3889,7 @@
         <v>44.780417479166672</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3867,7 +3903,7 @@
         <v>34.929931281249999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3881,7 +3917,7 @@
         <v>34.977382239583328</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3895,7 +3931,7 @@
         <v>33.605833333333337</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3909,7 +3945,7 @@
         <v>49.519791750000003</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3923,7 +3959,7 @@
         <v>34.884765625</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3937,7 +3973,7 @@
         <v>34.963575916666663</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3951,7 +3987,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3965,7 +4001,7 @@
         <v>29.270242499999998</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3979,7 +4015,7 @@
         <v>35.685509375000002</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3993,7 +4029,7 @@
         <v>30.826296875000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4007,7 +4043,7 @@
         <v>34.941444781249999</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4021,7 +4057,7 @@
         <v>43.290724537499997</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4035,7 +4071,7 @@
         <v>50.270417072916672</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4049,7 +4085,7 @@
         <v>34.576231999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4063,7 +4099,7 @@
         <v>46.293316816666668</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4077,7 +4113,7 @@
         <v>34.245382341666662</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4091,7 +4127,7 @@
         <v>44.61171134166667</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -4105,7 +4141,7 @@
         <v>42.835534087499987</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4119,7 +4155,7 @@
         <v>55.094791666666673</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4133,7 +4169,7 @@
         <v>34.971118875000002</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4147,7 +4183,7 @@
         <v>51.089435989583343</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4161,7 +4197,7 @@
         <v>45.176313204166661</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4175,7 +4211,7 @@
         <v>31.04461185000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4189,7 +4225,7 @@
         <v>47.39057605</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4203,7 +4239,7 @@
         <v>44.6331165</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4217,7 +4253,7 @@
         <v>35.126820000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4231,7 +4267,7 @@
         <v>46.161723541666667</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4245,7 +4281,7 @@
         <v>46.40645833333334</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4259,7 +4295,7 @@
         <v>34.930478708333339</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4273,7 +4309,7 @@
         <v>29.998251889583329</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4287,7 +4323,7 @@
         <v>31.933953599999999</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4301,7 +4337,7 @@
         <v>36.901689391666658</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4315,7 +4351,7 @@
         <v>24.888864000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4329,7 +4365,7 @@
         <v>34.993390724999998</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4343,7 +4379,7 @@
         <v>34.721358343749998</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4357,7 +4393,7 @@
         <v>30.857112000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4371,7 +4407,7 @@
         <v>34.794677291666673</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4385,7 +4421,7 @@
         <v>141.08094</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4399,7 +4435,7 @@
         <v>23.997312000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4413,7 +4449,7 @@
         <v>46.065770833333332</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4427,7 +4463,7 @@
         <v>45.603541666666658</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4441,7 +4477,7 @@
         <v>48.318135000000012</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4455,7 +4491,7 @@
         <v>37.43108190416666</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4469,7 +4505,7 @@
         <v>46.494241625000008</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4483,7 +4519,7 @@
         <v>47.329319249999998</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4497,7 +4533,7 @@
         <v>46.883411458333327</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4511,7 +4547,7 @@
         <v>47.501770833333332</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4525,7 +4561,7 @@
         <v>20.770429922916669</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4539,7 +4575,7 @@
         <v>33.936458333333327</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4553,7 +4589,7 @@
         <v>34.960412156250001</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4567,7 +4603,7 @@
         <v>46.061529291666659</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4581,7 +4617,7 @@
         <v>46.955097306250003</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4595,7 +4631,7 @@
         <v>33.573524562499998</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4609,7 +4645,7 @@
         <v>46.902209499999998</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4623,7 +4659,7 @@
         <v>31.875</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4637,7 +4673,7 @@
         <v>49.611490349999997</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4651,7 +4687,7 @@
         <v>34.02559632291667</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4665,7 +4701,7 @@
         <v>38.240625000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4679,7 +4715,7 @@
         <v>33.017618918750003</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4693,7 +4729,7 @@
         <v>34.990127600000001</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4707,7 +4743,7 @@
         <v>44.741033437499993</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4721,7 +4757,7 @@
         <v>34.974947537499993</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4735,7 +4771,7 @@
         <v>50.615410437500003</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4749,7 +4785,7 @@
         <v>38.790999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4763,7 +4799,7 @@
         <v>31.381765016666659</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4777,7 +4813,7 @@
         <v>34.658406999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4791,7 +4827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4805,7 +4841,7 @@
         <v>45.556808699999998</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4819,7 +4855,7 @@
         <v>41.904719999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4833,7 +4869,7 @@
         <v>38.0625</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4847,7 +4883,7 @@
         <v>41.994836366666661</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4861,7 +4897,7 @@
         <v>30.411287999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4875,7 +4911,7 @@
         <v>49.042243624999998</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4889,7 +4925,7 @@
         <v>45.582537452083329</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4903,7 +4939,7 @@
         <v>34.598853559895829</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4917,7 +4953,7 @@
         <v>34.867783812500001</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4931,7 +4967,7 @@
         <v>49.662451837500001</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4945,7 +4981,7 @@
         <v>51.933909493749987</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4959,7 +4995,7 @@
         <v>44.707201916666669</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4973,7 +5009,7 @@
         <v>47.649765350000003</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4987,7 +5023,7 @@
         <v>43.135464749999997</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -5001,7 +5037,7 @@
         <v>53.005595487500003</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -5015,7 +5051,7 @@
         <v>48.438939656249993</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -5029,7 +5065,7 @@
         <v>34.874965125000003</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -5043,7 +5079,7 @@
         <v>46.193223037499997</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -5057,7 +5093,7 @@
         <v>33.324704500000003</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -5071,7 +5107,7 @@
         <v>32.14284</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -5085,7 +5121,7 @@
         <v>49.072718093750012</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -5099,7 +5135,7 @@
         <v>34.790785791666657</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -5113,7 +5149,7 @@
         <v>44.946751464583343</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -5127,7 +5163,7 @@
         <v>44.791942822916667</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -5141,7 +5177,7 @@
         <v>34.974129187499997</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -5155,7 +5191,7 @@
         <v>59.19234197916667</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -5169,7 +5205,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -5183,7 +5219,7 @@
         <v>47.951169566666671</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -5197,7 +5233,7 @@
         <v>34.711080416666668</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -5211,7 +5247,7 @@
         <v>49.625</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -5225,7 +5261,7 @@
         <v>45.393341166666673</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -5239,7 +5275,7 @@
         <v>34.99158096875</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -5253,7 +5289,7 @@
         <v>248.59539375</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -5267,7 +5303,7 @@
         <v>44.347764000000012</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -5281,7 +5317,7 @@
         <v>44.945391562500014</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -5295,7 +5331,7 @@
         <v>48.54932465625</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -5309,7 +5345,7 @@
         <v>42.035673750000001</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -5323,7 +5359,7 @@
         <v>48.862109999999987</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -5337,7 +5373,7 @@
         <v>35.336727183333338</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -5351,7 +5387,7 @@
         <v>34.965144120833337</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -5365,7 +5401,7 @@
         <v>53.961999609374999</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -5379,7 +5415,7 @@
         <v>34.757703453125004</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -5393,7 +5429,7 @@
         <v>34.978883671875003</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -5407,7 +5443,7 @@
         <v>44.064623958333343</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -5421,7 +5457,7 @@
         <v>49.838610000000003</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -5435,7 +5471,7 @@
         <v>34.250006849999998</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -5449,7 +5485,7 @@
         <v>33.004544250000002</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5463,7 +5499,7 @@
         <v>48.041537854166677</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5477,7 +5513,7 @@
         <v>32.570510354166672</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5491,7 +5527,7 @@
         <v>34.81698024166667</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5505,7 +5541,7 @@
         <v>54.1455078125</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5519,7 +5555,7 @@
         <v>62.222500349999997</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5533,7 +5569,7 @@
         <v>34.695022312499987</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5547,7 +5583,7 @@
         <v>34.858959229166658</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5561,7 +5597,7 @@
         <v>35.412889768750013</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5575,7 +5611,7 @@
         <v>34.522111375000001</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5589,7 +5625,7 @@
         <v>34.589776000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5603,7 +5639,7 @@
         <v>44.999972999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5617,7 +5653,7 @@
         <v>33.976041666666667</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5631,7 +5667,7 @@
         <v>24.904040783333329</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5645,7 +5681,7 @@
         <v>34.813633987499998</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5659,7 +5695,7 @@
         <v>33.75083896666667</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5673,7 +5709,7 @@
         <v>44.995726637499999</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -5687,7 +5723,7 @@
         <v>34.965000000000003</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -5700,8 +5736,9 @@
       <c r="D146">
         <v>24.737159999999999</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="2"/>
+    </row>
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -5715,7 +5752,7 @@
         <v>18.950701124999998</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -5729,7 +5766,7 @@
         <v>45.555257983333341</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -5743,7 +5780,7 @@
         <v>45.527903575000003</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -5757,7 +5794,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -5771,7 +5808,7 @@
         <v>25.03044275000001</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -5785,7 +5822,7 @@
         <v>48.552325250000003</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -5799,7 +5836,7 @@
         <v>32.087767541666658</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -5813,7 +5850,7 @@
         <v>55.244878687500012</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -5827,7 +5864,7 @@
         <v>47.40625</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -5841,7 +5878,7 @@
         <v>46.010661652083343</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -5855,7 +5892,7 @@
         <v>34.809843945312501</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -5869,7 +5906,7 @@
         <v>34.976510416666663</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -5883,7 +5920,7 @@
         <v>32.959774743750003</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -5897,7 +5934,7 @@
         <v>45.842102583333329</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -5911,7 +5948,7 @@
         <v>37.681249999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -5925,7 +5962,7 @@
         <v>34.798385416666662</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -5939,7 +5976,7 @@
         <v>34.997149758333329</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -5953,7 +5990,7 @@
         <v>53.191706560416669</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -5967,7 +6004,7 @@
         <v>44.32773495</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -5981,7 +6018,7 @@
         <v>35.003274762499998</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -5995,7 +6032,7 @@
         <v>58.239144066666668</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -6009,7 +6046,7 @@
         <v>33.348510966145838</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6023,7 +6060,7 @@
         <v>20.025833333333331</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -6037,7 +6074,7 @@
         <v>34.953354916666669</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -6051,7 +6088,7 @@
         <v>44.844000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -6065,7 +6102,7 @@
         <v>44.652439304166663</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -6079,7 +6116,7 @@
         <v>44.536104000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -6093,7 +6130,7 @@
         <v>34.969737906250003</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6107,7 +6144,7 @@
         <v>40.676562500000003</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6121,7 +6158,7 @@
         <v>31.2456504375</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6135,7 +6172,7 @@
         <v>19.663616699999999</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6149,7 +6186,7 @@
         <v>47.181696222916663</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -6163,7 +6200,7 @@
         <v>62.808655941666657</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -6177,7 +6214,7 @@
         <v>44.494065866666659</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -6191,7 +6228,7 @@
         <v>31.913751999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -6205,7 +6242,7 @@
         <v>34.871759999999988</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -6219,7 +6256,7 @@
         <v>30.713575062499999</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -6233,7 +6270,7 @@
         <v>44.932790874999988</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -6247,7 +6284,7 @@
         <v>47.692848499999997</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -6261,7 +6298,7 @@
         <v>41.666600000000003</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -6274,8 +6311,9 @@
       <c r="D187">
         <v>254.07523311874999</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" s="2"/>
+    </row>
+    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -6289,7 +6327,7 @@
         <v>37.418793749999999</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -6303,7 +6341,7 @@
         <v>32.383554464583327</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -6317,7 +6355,7 @@
         <v>34.337811354166668</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -6331,7 +6369,7 @@
         <v>52.153704708333329</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -6345,7 +6383,7 @@
         <v>48.286659562500013</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -6359,7 +6397,7 @@
         <v>45.285911458333331</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -6373,7 +6411,7 @@
         <v>48.203000000000003</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -6387,7 +6425,7 @@
         <v>34.974737687500003</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -6401,7 +6439,7 @@
         <v>34.703783630208328</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -6415,7 +6453,7 @@
         <v>32.589150843749998</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -6429,7 +6467,7 @@
         <v>33.671839083333339</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -6443,7 +6481,7 @@
         <v>36.337735539583328</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -6457,7 +6495,7 @@
         <v>34.604597604166663</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -6471,7 +6509,7 @@
         <v>44.451983650000003</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -6485,7 +6523,7 @@
         <v>47.611639108333343</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -6499,7 +6537,7 @@
         <v>58.278513150000009</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -6513,7 +6551,7 @@
         <v>39.111072</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -6527,7 +6565,7 @@
         <v>46.164796160416657</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -6541,7 +6579,7 @@
         <v>34.954999999999998</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -6555,7 +6593,7 @@
         <v>32.459723066666669</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -6569,7 +6607,7 @@
         <v>56.368338750000007</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -6583,7 +6621,7 @@
         <v>44.999952</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -6597,7 +6635,7 @@
         <v>44.795000000000002</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -6611,7 +6649,7 @@
         <v>50.785810750000003</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -6625,7 +6663,7 @@
         <v>34.9462890625</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -6639,7 +6677,7 @@
         <v>47.605316331250002</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -6653,7 +6691,7 @@
         <v>38.319276000000002</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -6667,7 +6705,7 @@
         <v>39.415471343749999</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -6681,7 +6719,7 @@
         <v>45.256130525000003</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -6695,7 +6733,7 @@
         <v>30.266291172916659</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -6709,7 +6747,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -6723,7 +6761,7 @@
         <v>34.999965583333328</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -6737,7 +6775,7 @@
         <v>199.426828</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -6751,7 +6789,7 @@
         <v>49.142646402083329</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -6765,7 +6803,7 @@
         <v>28.226991949999999</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -6779,7 +6817,7 @@
         <v>138.13762</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -6793,7 +6831,7 @@
         <v>37.697869687500003</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -6807,7 +6845,7 @@
         <v>46.731553322916668</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -6821,7 +6859,7 @@
         <v>45.016529068750003</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -6835,7 +6873,7 @@
         <v>34.834021625000013</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -6849,7 +6887,7 @@
         <v>36.346648000000002</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -6863,7 +6901,7 @@
         <v>34.877874249999998</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -6877,7 +6915,7 @@
         <v>47.174016927083343</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -6891,7 +6929,7 @@
         <v>42.082455424999999</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -6905,7 +6943,7 @@
         <v>47.894861445833342</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -6919,7 +6957,7 @@
         <v>55.58902346666666</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -6933,7 +6971,7 @@
         <v>34.524849699999997</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -6947,7 +6985,7 @@
         <v>30.862594866666669</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -6961,7 +6999,7 @@
         <v>34.498958333333327</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -6975,7 +7013,7 @@
         <v>223.2059205416667</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -6989,7 +7027,7 @@
         <v>31.875</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -7003,7 +7041,7 @@
         <v>39.99445755208334</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -7017,7 +7055,7 @@
         <v>57.68920067291667</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -7031,7 +7069,7 @@
         <v>34.703961249999999</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -7045,7 +7083,7 @@
         <v>33.856250000000003</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -7059,7 +7097,7 @@
         <v>34.656046833333328</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -7073,7 +7111,7 @@
         <v>46.917276348958353</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -7087,7 +7125,7 @@
         <v>44.667200000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -7101,7 +7139,7 @@
         <v>45.923249531250001</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -7115,7 +7153,7 @@
         <v>33.745823085937502</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -7129,7 +7167,7 @@
         <v>46.098080764583337</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -7143,7 +7181,7 @@
         <v>29.60071504166666</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -7157,7 +7195,7 @@
         <v>32.990048020833328</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -7171,7 +7209,7 @@
         <v>37.140109606770842</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -7185,7 +7223,7 @@
         <v>44.144894489583343</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -7199,7 +7237,7 @@
         <v>61.95068359375</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -7213,7 +7251,7 @@
         <v>27.567540000000001</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -7227,7 +7265,7 @@
         <v>44.978930875000003</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -7241,7 +7279,7 @@
         <v>27.745640000000002</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -7255,7 +7293,7 @@
         <v>34.538249437499999</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -7269,7 +7307,7 @@
         <v>39.745033168750012</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -7283,7 +7321,7 @@
         <v>44.999549999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -7297,7 +7335,7 @@
         <v>29.40794767083333</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -7311,7 +7349,7 @@
         <v>33.916543500000003</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -7325,7 +7363,7 @@
         <v>45.21965325</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -7339,7 +7377,7 @@
         <v>44.898191924999999</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -7353,7 +7391,7 @@
         <v>54.140047604166668</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -7367,7 +7405,7 @@
         <v>44.671771166666673</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -7381,7 +7419,7 @@
         <v>34.650964750000007</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -7395,7 +7433,7 @@
         <v>194.10587000000001</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -7409,7 +7447,7 @@
         <v>39.045076416666667</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -7423,7 +7461,7 @@
         <v>29.486641250000002</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -7437,7 +7475,7 @@
         <v>47.288960354166683</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -7451,7 +7489,7 @@
         <v>46.237034814583339</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -7465,7 +7503,7 @@
         <v>35.053811099999997</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -7479,7 +7517,7 @@
         <v>23.208322889583329</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -7493,7 +7531,7 @@
         <v>30.554765458333328</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -7507,7 +7545,7 @@
         <v>16.12105866666667</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -7521,7 +7559,7 @@
         <v>35.282766891666668</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -7535,7 +7573,7 @@
         <v>39.547877200000002</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -7549,7 +7587,7 @@
         <v>28.600246106250001</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -7563,7 +7601,7 @@
         <v>38.499990625000002</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -7577,7 +7615,7 @@
         <v>43.732100625000008</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -7590,8 +7628,9 @@
       <c r="D281">
         <v>44.519081008333337</v>
       </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E281" s="3"/>
+    </row>
+    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -7605,7 +7644,7 @@
         <v>264.1146559</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -7619,7 +7658,7 @@
         <v>29.61298457916666</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -7633,7 +7672,7 @@
         <v>35.989121687500003</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -7647,7 +7686,7 @@
         <v>27.58624</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -7661,7 +7700,7 @@
         <v>48.004145833333332</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -7675,7 +7714,7 @@
         <v>34.939446250000003</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -7689,7 +7728,7 @@
         <v>36.056621500000013</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -7703,7 +7742,7 @@
         <v>45.530455183333338</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -7717,7 +7756,7 @@
         <v>20.698211624999999</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -7731,7 +7770,7 @@
         <v>48.93352591666666</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -7745,7 +7784,7 @@
         <v>35.695512000000001</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -7759,7 +7798,7 @@
         <v>35.8330078125</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -7773,7 +7812,7 @@
         <v>45.679138710416659</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -7787,7 +7826,7 @@
         <v>34.692333083333331</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -7801,7 +7840,7 @@
         <v>45.078170204166668</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -7815,7 +7854,7 @@
         <v>42.253500000000003</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -7829,7 +7868,7 @@
         <v>33.637329000000001</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -7843,7 +7882,7 @@
         <v>25.714248000000001</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -7857,7 +7896,7 @@
         <v>33.021000000000001</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -7871,7 +7910,7 @@
         <v>48.001204549999997</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -7885,7 +7924,7 @@
         <v>34.871263300000003</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -7899,7 +7938,7 @@
         <v>31.983494151041668</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -7913,7 +7952,7 @@
         <v>54.652454010416683</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -7927,7 +7966,7 @@
         <v>31.022043312499999</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -7941,7 +7980,7 @@
         <v>37.682812499999997</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -7955,7 +7994,7 @@
         <v>47.080467284374997</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -7969,7 +8008,7 @@
         <v>50.541643524999998</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -7983,7 +8022,7 @@
         <v>65.854166666666657</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -7997,7 +8036,7 @@
         <v>46.782371249999997</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -8011,7 +8050,7 @@
         <v>28.602080183333339</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -8025,7 +8064,7 @@
         <v>17.588872899999998</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -8039,7 +8078,7 @@
         <v>51.651041666666657</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -8053,7 +8092,7 @@
         <v>35.817393166666662</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -8067,7 +8106,7 @@
         <v>53.861058749999998</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -8081,7 +8120,7 @@
         <v>46.133607712499987</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -8095,7 +8134,7 @@
         <v>38.249961749999997</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -8109,7 +8148,7 @@
         <v>32.878717095833331</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -8123,7 +8162,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -8137,7 +8176,7 @@
         <v>54.431317177083343</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -8151,7 +8190,7 @@
         <v>59.317557293749999</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -8165,7 +8204,7 @@
         <v>34.597249900000001</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -8179,7 +8218,7 @@
         <v>32.992411433333331</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -8193,7 +8232,7 @@
         <v>44.981783</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -8207,7 +8246,7 @@
         <v>45.005299479166673</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -8221,7 +8260,7 @@
         <v>30.668177368750001</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -8235,7 +8274,7 @@
         <v>25.64519349375</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -8249,7 +8288,7 @@
         <v>46.003229166666671</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -8263,7 +8302,7 @@
         <v>34.9375</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -8277,7 +8316,7 @@
         <v>44.648212083333327</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -8291,7 +8330,7 @@
         <v>39.652164000000013</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -8305,7 +8344,7 @@
         <v>12.14790533333333</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -8319,7 +8358,7 @@
         <v>63.660080000000008</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -8333,7 +8372,7 @@
         <v>46.169546841666659</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -8347,7 +8386,7 @@
         <v>32.272304216666669</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -8361,7 +8400,7 @@
         <v>63.763427734375</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -8375,7 +8414,7 @@
         <v>34.9541015625</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -8389,7 +8428,7 @@
         <v>45.587817108333333</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -8403,7 +8442,7 @@
         <v>33.931074023437503</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -8417,7 +8456,7 @@
         <v>48.956000000000003</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -8431,7 +8470,7 @@
         <v>46.61328125</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -8445,7 +8484,7 @@
         <v>46.838212624999997</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -8459,7 +8498,7 @@
         <v>48.773412287500001</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -8473,7 +8512,7 @@
         <v>44.551360625000001</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -8487,7 +8526,7 @@
         <v>36.166632</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -8501,7 +8540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -8515,7 +8554,7 @@
         <v>42.650003454166672</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -8529,7 +8568,7 @@
         <v>71.999963999999991</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -8543,7 +8582,7 @@
         <v>44.999955</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -8557,7 +8596,7 @@
         <v>42.092044374999993</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -8570,8 +8609,9 @@
       <c r="D351">
         <v>26.024076000000001</v>
       </c>
-    </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E351" s="2"/>
+    </row>
+    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -8585,7 +8625,7 @@
         <v>53.248385416666657</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -8599,7 +8639,7 @@
         <v>34.783837343750001</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -8613,7 +8653,7 @@
         <v>34.77734375</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -8627,7 +8667,7 @@
         <v>45.447871218750002</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -8641,7 +8681,7 @@
         <v>35.569009049999998</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -8655,7 +8695,7 @@
         <v>46.091041666666669</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -8669,7 +8709,7 @@
         <v>40.989306889583332</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -8683,7 +8723,7 @@
         <v>45.99583333333333</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -8697,7 +8737,7 @@
         <v>33.09731816041667</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -8711,7 +8751,7 @@
         <v>48.904830583333343</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -8725,7 +8765,7 @@
         <v>34.9140625</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -8739,7 +8779,7 @@
         <v>49.488210549999998</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -8753,7 +8793,7 @@
         <v>32.797418233333339</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -8767,7 +8807,7 @@
         <v>42.523696614583329</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -8781,7 +8821,7 @@
         <v>45.00382161458333</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -8795,7 +8835,7 @@
         <v>45.185781249999998</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -8809,7 +8849,7 @@
         <v>167.43528341666669</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -8823,7 +8863,7 @@
         <v>167.7751545739583</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -8837,7 +8877,7 @@
         <v>39.844592020833332</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -8851,7 +8891,7 @@
         <v>46.003136166666657</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -8865,7 +8905,7 @@
         <v>38.499493249999993</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -8879,7 +8919,7 @@
         <v>46.565278329166667</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -8893,7 +8933,7 @@
         <v>47.379643281249997</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -8907,7 +8947,7 @@
         <v>30.419879156250001</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -8921,7 +8961,7 @@
         <v>34.05833333333333</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -8935,7 +8975,7 @@
         <v>18.79626692708333</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -8949,7 +8989,7 @@
         <v>44.999974500000008</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -8963,7 +9003,7 @@
         <v>24.742239999999999</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -8977,7 +9017,7 @@
         <v>45.643412441666683</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -8991,7 +9031,7 @@
         <v>48.077527812500001</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -9005,7 +9045,7 @@
         <v>27.789432000000001</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -9019,7 +9059,7 @@
         <v>34.981644350000003</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -9033,7 +9073,7 @@
         <v>47.333287499999997</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -9047,7 +9087,7 @@
         <v>42.424999999999997</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>384</v>
       </c>
@@ -9061,7 +9101,7 @@
         <v>54.790768174999997</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -9075,7 +9115,7 @@
         <v>31.155096077083339</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -9089,7 +9129,7 @@
         <v>32.645229499999999</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -9103,7 +9143,7 @@
         <v>34.993846124999997</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -9117,7 +9157,7 @@
         <v>46.274200695833329</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -9131,7 +9171,7 @@
         <v>49.754477937499999</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -9145,7 +9185,7 @@
         <v>34.938201041666673</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -9159,7 +9199,7 @@
         <v>34.867269374999999</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>392</v>
       </c>
@@ -9173,7 +9213,7 @@
         <v>39.126953125</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -9187,7 +9227,7 @@
         <v>44.98</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -9201,7 +9241,7 @@
         <v>45.4407675</v>
       </c>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -9215,7 +9255,7 @@
         <v>34.877611908333343</v>
       </c>
     </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -9229,7 +9269,7 @@
         <v>34.976451062499997</v>
       </c>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -9243,7 +9283,7 @@
         <v>34.945755758333327</v>
       </c>
     </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -9257,7 +9297,7 @@
         <v>43.333316000000003</v>
       </c>
     </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -9271,7 +9311,7 @@
         <v>41.412056666666672</v>
       </c>
     </row>
-    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -9285,7 +9325,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>401</v>
       </c>
@@ -9299,7 +9339,7 @@
         <v>30.31172590625</v>
       </c>
     </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>402</v>
       </c>
@@ -9313,7 +9353,7 @@
         <v>29.561552816666669</v>
       </c>
     </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>403</v>
       </c>
@@ -9327,7 +9367,7 @@
         <v>52.968454916666673</v>
       </c>
     </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>404</v>
       </c>
@@ -9341,7 +9381,7 @@
         <v>35.015050937500007</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -9355,7 +9395,7 @@
         <v>46.356521729166673</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -9369,7 +9409,7 @@
         <v>34.604366499999998</v>
       </c>
     </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>407</v>
       </c>
@@ -9383,7 +9423,7 @@
         <v>27.690356925</v>
       </c>
     </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>408</v>
       </c>
@@ -9397,7 +9437,7 @@
         <v>36.06640625</v>
       </c>
     </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>409</v>
       </c>
@@ -9411,7 +9451,7 @@
         <v>45.684227999999997</v>
       </c>
     </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -9424,8 +9464,9 @@
       <c r="D412">
         <v>111.0701211666666</v>
       </c>
-    </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E412" s="2"/>
+    </row>
+    <row r="413" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>411</v>
       </c>
@@ -9439,7 +9480,7 @@
         <v>171.80527044791671</v>
       </c>
     </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -9453,7 +9494,7 @@
         <v>36.269755755208337</v>
       </c>
     </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>413</v>
       </c>
@@ -9467,7 +9508,7 @@
         <v>36.197060968750002</v>
       </c>
     </row>
-    <row r="416" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>414</v>
       </c>
@@ -9481,7 +9522,7 @@
         <v>24.9946178625</v>
       </c>
     </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>415</v>
       </c>
@@ -9495,7 +9536,7 @@
         <v>46.63671875</v>
       </c>
     </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -9509,7 +9550,7 @@
         <v>44.999444999999987</v>
       </c>
     </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>417</v>
       </c>
@@ -9523,7 +9564,7 @@
         <v>44.997395833333329</v>
       </c>
     </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>418</v>
       </c>
@@ -9537,7 +9578,7 @@
         <v>43.942999999999998</v>
       </c>
     </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>419</v>
       </c>
@@ -9551,7 +9592,7 @@
         <v>39.998333333333328</v>
       </c>
     </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -9565,7 +9606,7 @@
         <v>30.983857024999999</v>
       </c>
     </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>421</v>
       </c>
@@ -9579,7 +9620,7 @@
         <v>52.221995514583341</v>
       </c>
     </row>
-    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>422</v>
       </c>
@@ -9593,7 +9634,7 @@
         <v>71.510357552083335</v>
       </c>
     </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -9607,7 +9648,7 @@
         <v>38.765345850000003</v>
       </c>
     </row>
-    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>424</v>
       </c>
@@ -9621,7 +9662,7 @@
         <v>46.861328125</v>
       </c>
     </row>
-    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>425</v>
       </c>
@@ -9635,7 +9676,7 @@
         <v>34.931604624999999</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>426</v>
       </c>
@@ -9649,7 +9690,7 @@
         <v>41.822110008333333</v>
       </c>
     </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>427</v>
       </c>
@@ -9663,7 +9704,7 @@
         <v>32.995571737500001</v>
       </c>
     </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>428</v>
       </c>
@@ -9677,7 +9718,7 @@
         <v>37.498437500000001</v>
       </c>
     </row>
-    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>429</v>
       </c>
@@ -9690,8 +9731,9 @@
       <c r="D431">
         <v>46.827649937499999</v>
       </c>
-    </row>
-    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E431" s="2"/>
+    </row>
+    <row r="432" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -9705,7 +9747,7 @@
         <v>35.861148749999998</v>
       </c>
     </row>
-    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>431</v>
       </c>
@@ -9719,7 +9761,7 @@
         <v>57.781211614583341</v>
       </c>
     </row>
-    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -9733,7 +9775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>433</v>
       </c>
@@ -9747,7 +9789,7 @@
         <v>33.976520179166663</v>
       </c>
     </row>
-    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>434</v>
       </c>
@@ -9761,7 +9803,7 @@
         <v>27.204816874999999</v>
       </c>
     </row>
-    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>435</v>
       </c>
@@ -9775,7 +9817,7 @@
         <v>42.86328125</v>
       </c>
     </row>
-    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>436</v>
       </c>
@@ -9789,7 +9831,7 @@
         <v>46.004062500000003</v>
       </c>
     </row>
-    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>437</v>
       </c>
@@ -9803,7 +9845,7 @@
         <v>45.923249531250001</v>
       </c>
     </row>
-    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>438</v>
       </c>
@@ -9817,7 +9859,7 @@
         <v>47.240062999999992</v>
       </c>
     </row>
-    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>439</v>
       </c>
@@ -9831,7 +9873,7 @@
         <v>43.608963850000002</v>
       </c>
     </row>
-    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>440</v>
       </c>
@@ -9845,7 +9887,7 @@
         <v>44.999932499999993</v>
       </c>
     </row>
-    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>441</v>
       </c>

</xml_diff>

<commit_message>
Delete of 3/4 songs
</commit_message>
<xml_diff>
--- a/dataset/songs_with_signature_and_length.xlsx
+++ b/dataset/songs_with_signature_and_length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\Documents\GitHub\Tresillo\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B74174E-DF95-4920-8CD2-A8F20676ADB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3084CE7F-F666-41B0-9090-AB8B89DF473A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="459">
   <si>
     <t>name</t>
   </si>
@@ -3176,21 +3176,6 @@
   </si>
   <si>
     <t>Spalte1</t>
-  </si>
-  <si>
-    <t>Spalte2</t>
-  </si>
-  <si>
-    <t>Summe</t>
-  </si>
-  <si>
-    <t>Mittelwert</t>
-  </si>
-  <si>
-    <t>Laufende Summe</t>
-  </si>
-  <si>
-    <t>Anzahl</t>
   </si>
 </sst>
 </file>
@@ -3412,10 +3397,12 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1BC977F-93A7-4443-B601-8EA545A39641}" name="Tabelle1" displayName="Tabelle1" ref="A1:D444" totalsRowCount="1" headerRowDxfId="2">
   <autoFilter ref="A1:D443" xr:uid="{5A276807-760A-4EC0-83F2-9F298F09E7B0}">
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="lessThan" val="25"/>
-      </customFilters>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="{1: '12/8'}"/>
+        <filter val="{1: '3/4'}"/>
+        <filter val="{1: '6/8'}"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D443">
@@ -3755,7 +3742,7 @@
   <dimension ref="A1:E444"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:C434"/>
+      <selection activeCell="B337" sqref="B337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3821,7 +3808,7 @@
         <v>25.714248000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>349</v>
       </c>
@@ -4409,7 +4396,7 @@
         <v>31.933953599999999</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4493,7 +4480,7 @@
         <v>32.383554464583327</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4619,7 +4606,7 @@
         <v>32.990048020833328</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4717,7 +4704,7 @@
         <v>33.09731816041667</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>98</v>
       </c>
@@ -5729,7 +5716,7 @@
         <v>34.9541015625</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5814,7 +5801,7 @@
       </c>
       <c r="E146" s="2"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -6122,7 +6109,7 @@
         <v>35.053811099999997</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6234,7 +6221,7 @@
         <v>35.685509375000002</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6571,7 +6558,7 @@
         <v>38.0625</v>
       </c>
     </row>
-    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>70</v>
       </c>
@@ -7229,7 +7216,7 @@
         <v>44.494065866666659</v>
       </c>
     </row>
-    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>279</v>
       </c>
@@ -7579,7 +7566,7 @@
         <v>44.997395833333329</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -7607,7 +7594,7 @@
         <v>44.999444999999987</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -7818,7 +7805,7 @@
         <v>45.185781249999998</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -8126,7 +8113,7 @@
         <v>46.003136166666657</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -8406,7 +8393,7 @@
         <v>46.565278329166667</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -8476,7 +8463,7 @@
         <v>46.782371249999997</v>
       </c>
     </row>
-    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>429</v>
       </c>
@@ -9038,7 +9025,7 @@
         <v>48.93352591666666</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -9066,7 +9053,7 @@
         <v>48.956000000000003</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -9585,7 +9572,7 @@
         <v>57.68920067291667</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>414</v>
       </c>
@@ -9655,7 +9642,7 @@
         <v>58.278513150000009</v>
       </c>
     </row>
-    <row r="421" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>105</v>
       </c>
@@ -9795,7 +9782,7 @@
         <v>71.999963999999991</v>
       </c>
     </row>
-    <row r="431" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>410</v>
       </c>
@@ -9838,7 +9825,7 @@
         <v>141.08094</v>
       </c>
     </row>
-    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -9950,7 +9937,7 @@
         <v>248.59539375</v>
       </c>
     </row>
-    <row r="442" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>185</v>
       </c>
@@ -9982,7 +9969,7 @@
       <c r="A444" s="4"/>
       <c r="D444">
         <f>SUBTOTAL(101,Tabelle1[length])</f>
-        <v>20.837379651102939</v>
+        <v>70.890110301157392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>